<commit_message>
cleaning rnaSample 06.12.19 hbrown
</commit_message>
<xml_diff>
--- a/rnaSample/rnaSample_hbrown_06.12.19.xlsx
+++ b/rnaSample/rnaSample_hbrown_06.12.19.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">harvester</t>
   </si>
   <si>
-    <t xml:space="preserve">biosampleNumber</t>
+    <t xml:space="preserve">bioSampleNumber</t>
   </si>
   <si>
     <t xml:space="preserve">rnaDate</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">2d 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Trizol</t>
+    <t xml:space="preserve">TRIzol</t>
   </si>
   <si>
     <t xml:space="preserve">2d 2</t>
@@ -156,7 +156,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -196,13 +196,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -249,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,10 +265,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -302,10 +291,10 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H27"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2:G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.61"/>
   </cols>
@@ -381,10 +370,11 @@
       <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="7" t="b">
+      <c r="G2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I2" s="1"/>
@@ -425,10 +415,11 @@
       <c r="F3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="7" t="b">
+      <c r="G3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -451,10 +442,11 @@
       <c r="F4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="7" t="b">
+      <c r="G4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -477,10 +469,11 @@
       <c r="F5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="7" t="b">
+      <c r="G5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -503,10 +496,11 @@
       <c r="F6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="7" t="b">
+      <c r="G6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -529,10 +523,11 @@
       <c r="F7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="7" t="b">
+      <c r="G7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -555,10 +550,11 @@
       <c r="F8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="7" t="b">
+      <c r="G8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -581,10 +577,11 @@
       <c r="F9" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="7" t="b">
+      <c r="G9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -607,10 +604,11 @@
       <c r="F10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="7" t="b">
+      <c r="G10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -633,10 +631,11 @@
       <c r="F11" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="7" t="b">
+      <c r="G11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -659,10 +658,11 @@
       <c r="F12" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="7" t="b">
+      <c r="G12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -685,10 +685,11 @@
       <c r="F13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="7" t="b">
+      <c r="G13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -711,10 +712,11 @@
       <c r="F14" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="7" t="b">
+      <c r="G14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -737,10 +739,11 @@
       <c r="F15" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="7" t="b">
+      <c r="G15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -763,10 +766,11 @@
       <c r="F16" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="7" t="b">
+      <c r="G16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -789,10 +793,11 @@
       <c r="F17" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="7" t="b">
+      <c r="G17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -815,10 +820,11 @@
       <c r="F18" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="7" t="b">
+      <c r="G18" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -841,10 +847,11 @@
       <c r="F19" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="7" t="b">
+      <c r="G19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -867,10 +874,11 @@
       <c r="F20" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="7" t="b">
+      <c r="G20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -893,10 +901,11 @@
       <c r="F21" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="7" t="b">
+      <c r="G21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -919,10 +928,11 @@
       <c r="F22" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="7" t="b">
+      <c r="G22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -945,10 +955,11 @@
       <c r="F23" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="7" t="b">
+      <c r="G23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -971,10 +982,11 @@
       <c r="F24" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="7" t="b">
+      <c r="G24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -997,10 +1009,11 @@
       <c r="F25" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="7" t="b">
+      <c r="G25" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1023,10 +1036,11 @@
       <c r="F26" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="7" t="b">
+      <c r="G26" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1049,20 +1063,15 @@
       <c r="F27" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="7" t="b">
+      <c r="G27" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G27" type="list">
-      <formula1>"DirectZol,Trizol"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>